<commit_message>
Changed the report file
</commit_message>
<xml_diff>
--- a/ReportData.xlsx
+++ b/ReportData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Sr. No</t>
   </si>
@@ -82,13 +82,34 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>Actual Grade</t>
+  </si>
+  <si>
+    <t>Predicted Grade</t>
+  </si>
+  <si>
+    <t>Grade Distribution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,16 +117,76 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -113,24 +194,112 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -442,18 +611,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D10" sqref="D10:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="15" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +634,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -469,7 +642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -477,7 +650,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -485,7 +658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -493,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -501,7 +674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -509,84 +682,281 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D10" s="3" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q9" s="9"/>
+      <c r="R9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="Q10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D12" s="1" t="s">
+      <c r="L11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R11" s="7">
+        <v>13</v>
+      </c>
+      <c r="S11" s="8">
+        <v>1</v>
+      </c>
+      <c r="T11" s="2">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D13" s="1" t="s">
+      <c r="L12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.85211809999999999</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.80146790000000001</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R12" s="8">
+        <v>4</v>
+      </c>
+      <c r="S12" s="7">
+        <v>24</v>
+      </c>
+      <c r="T12" s="8">
+        <v>2</v>
+      </c>
+      <c r="U12" s="2">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="D13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="2">
         <v>130</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2">
         <v>103</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="2">
         <v>62</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="2">
         <v>60</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="2">
         <v>40</v>
       </c>
+      <c r="L13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0.85211809999999999</v>
+      </c>
+      <c r="N13" s="3">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.90486800000000001</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="8">
+        <v>7</v>
+      </c>
+      <c r="T13" s="7">
+        <v>20</v>
+      </c>
+      <c r="U13" s="8">
+        <v>15</v>
+      </c>
+      <c r="V13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="L14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.80146790000000001</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0.90486800000000001</v>
+      </c>
+      <c r="O14" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R14" s="2">
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <v>0</v>
+      </c>
+      <c r="T14" s="8">
+        <v>10</v>
+      </c>
+      <c r="U14" s="7">
+        <v>32</v>
+      </c>
+      <c r="V14" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q15" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R15" s="2">
+        <v>0</v>
+      </c>
+      <c r="S15" s="2">
+        <v>0</v>
+      </c>
+      <c r="T15" s="2">
+        <v>0</v>
+      </c>
+      <c r="U15" s="8">
+        <v>6</v>
+      </c>
+      <c r="V15" s="7">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E17" s="11"/>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="G20" s="6"/>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="G26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="D10:I10"/>
+    <mergeCell ref="K19:O19"/>
+    <mergeCell ref="R9:V9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>